<commit_message>
sync button on upload, dynamic template, flush method msg added
</commit_message>
<xml_diff>
--- a/web/upload/template.xlsx
+++ b/web/upload/template.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="19">
   <si>
     <t>districtCode</t>
   </si>
@@ -72,9 +72,6 @@
   </si>
   <si>
     <t>campaignId</t>
-  </si>
-  <si>
-    <t>id</t>
   </si>
 </sst>
 </file>
@@ -413,7 +410,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:T1"/>
+  <dimension ref="A1:S1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -421,7 +418,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" spans="1:20">
+    <row r="1" spans="1:19">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -478,9 +475,6 @@
       </c>
       <c r="S1" t="s">
         <v>18</v>
-      </c>
-      <c r="T1" t="s">
-        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>